<commit_message>
chnages for saving best simclr model
</commit_message>
<xml_diff>
--- a/images/ca_data_collection.xlsx
+++ b/images/ca_data_collection.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Desktop/MIDS_TPG/W210/capstone_fall20_irrigation/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBDE350-959C-B741-9EF1-45D5EDF287C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B17CB-B8AD-704F-8B9B-CBF790F4C393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57680" yWindow="14800" windowWidth="28040" windowHeight="17440" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
+    <workbookView xWindow="52780" yWindow="5400" windowWidth="36260" windowHeight="28860" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="20">
   <si>
     <t>LATITUDE</t>
   </si>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +112,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B11D730-724F-C64E-B450-810506062CA1}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,8 +963,11 @@
       <c r="B34">
         <v>-121.375</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>17</v>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -968,8 +977,11 @@
       <c r="B35">
         <v>-121.125</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>17</v>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1054,8 +1066,11 @@
       <c r="B42">
         <v>-120.875</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>17</v>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1130,7 +1145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>37.625</v>
       </c>
@@ -1141,7 +1156,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>37.875</v>
       </c>
@@ -1152,18 +1167,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>37.875</v>
       </c>
       <c r="B51">
         <v>-121.125</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>37.875</v>
       </c>
@@ -1174,7 +1192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>37.875</v>
       </c>
@@ -1185,18 +1203,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>38.125</v>
       </c>
       <c r="B54">
         <v>-121.375</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>38.125</v>
       </c>
@@ -1207,29 +1228,35 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>38.125</v>
       </c>
       <c r="B56">
         <v>-120.875</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>38.125</v>
       </c>
       <c r="B57">
         <v>-120.625</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>38.375</v>
       </c>
@@ -1240,7 +1267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>38.375</v>
       </c>
@@ -1251,7 +1278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>38.375</v>
       </c>
@@ -1262,7 +1289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>38.375</v>
       </c>
@@ -1273,13 +1300,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>COUNT(A2:A61)*644</f>
         <v>38640</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
evaluation of different finetune strategies
</commit_message>
<xml_diff>
--- a/images/ca_data_collection.xlsx
+++ b/images/ca_data_collection.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Desktop/MIDS_TPG/W210/capstone_fall20_irrigation/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B722C8-174F-1446-B191-109CAB8F79C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F1222A-18F5-5846-945C-4EF56C4DEBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62300" yWindow="4700" windowWidth="36260" windowHeight="28860" activeTab="2" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
+    <workbookView xWindow="7140" yWindow="1360" windowWidth="36260" windowHeight="28340" activeTab="2" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CA_Data_Collection" sheetId="1" r:id="rId1"/>
     <sheet name="ValidationAUC" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="33">
   <si>
     <t>LATITUDE</t>
   </si>
@@ -89,9 +89,6 @@
     <t>DECEMBER</t>
   </si>
   <si>
-    <t>MARIA</t>
-  </si>
-  <si>
     <t>APRIL</t>
   </si>
   <si>
@@ -120,6 +117,24 @@
   </si>
   <si>
     <t>Supervised - 100% Positive Class</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 25% Intensity</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 75% Intensity</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 100% Intensity</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - H1@512</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - H2@128</t>
   </si>
 </sst>
 </file>
@@ -175,13 +190,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -221,7 +235,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -234,11 +248,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Preliminary Comparison of Validation</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> Set Results</a:t>
             </a:r>
           </a:p>
@@ -257,7 +279,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -345,7 +367,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
@@ -366,7 +388,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
@@ -412,10 +434,10 @@
                   <c:v>Supervised - 13% Positive Class</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Supervised - 3% Positive Class</c:v>
+                  <c:v>SimCLR Pretrain (20% training set) and Finetuned - 13% Positive Class</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SimCLR Pretrain (20% training set) and Finetuned - 13% Positive Class</c:v>
+                  <c:v>Supervised - 3% Positive Class</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class</c:v>
@@ -439,13 +461,13 @@
                   <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.91500000000000004</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9</c:v>
+                  <c:v>0.91400000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,10 +521,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -542,6 +561,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Validation Set AUC </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -558,12 +636,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -621,6 +696,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1211,6 +1287,119 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76994</cdr:x>
+      <cdr:y>0.17646</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.86799</cdr:x>
+      <cdr:y>0.23927</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A5BCAB-9A70-D846-962A-243601A5B8A0}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="5400000">
+          <a:off x="6904278" y="880750"/>
+          <a:ext cx="394633" cy="850254"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.77367</cdr:x>
+      <cdr:y>0.25241</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88868</cdr:x>
+      <cdr:y>0.36319</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{444D3236-8A03-0A44-8237-8BB186E4F9D1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6708758" y="1585706"/>
+          <a:ext cx="997345" cy="695988"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>SimCLR     Pre-training</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> Benefit</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1512,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B11D730-724F-C64E-B450-810506062CA1}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView topLeftCell="A32" zoomScale="135" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1737,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1593,7 +1782,7 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1806,8 +1995,8 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>18</v>
+      <c r="E20" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1879,7 +2068,7 @@
       <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2030,8 +2219,11 @@
       <c r="B36">
         <v>-120.875</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>17</v>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2041,8 +2233,11 @@
       <c r="B37">
         <v>-120.625</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>17</v>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2080,8 +2275,11 @@
       <c r="B40">
         <v>-121.375</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>17</v>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2091,11 +2289,14 @@
       <c r="B41">
         <v>-121.125</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>17</v>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2119,8 +2320,11 @@
       <c r="B43">
         <v>-120.625</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>17</v>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2134,7 +2338,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2158,8 +2362,11 @@
       <c r="B46">
         <v>-121.375</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>17</v>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2169,7 +2376,10 @@
       <c r="B47">
         <v>-121.125</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2180,8 +2390,11 @@
       <c r="B48">
         <v>-120.875</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>17</v>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2191,8 +2404,11 @@
       <c r="B49">
         <v>-120.625</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>17</v>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2202,8 +2418,11 @@
       <c r="B50">
         <v>-121.375</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>17</v>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2227,8 +2446,11 @@
       <c r="B52">
         <v>-120.875</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>17</v>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2238,8 +2460,11 @@
       <c r="B53">
         <v>-120.625</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>17</v>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2263,8 +2488,11 @@
       <c r="B55">
         <v>-121.125</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>17</v>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2302,8 +2530,11 @@
       <c r="B58">
         <v>-121.375</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>17</v>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2313,8 +2544,11 @@
       <c r="B59">
         <v>-121.125</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>17</v>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2324,7 +2558,10 @@
       <c r="B60">
         <v>-120.875</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2335,8 +2572,11 @@
       <c r="B61">
         <v>-120.625</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>17</v>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2353,29 +2593,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BC90CD-1B1D-A349-9236-A951D1CE880F}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0.97499999999999998</v>
@@ -2383,7 +2623,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0.95</v>
@@ -2391,7 +2631,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0.91</v>
@@ -2399,26 +2639,74 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>0.91500000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>0.91500000000000004</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>0.9</v>
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0.91300000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready for final pretraining
</commit_message>
<xml_diff>
--- a/images/ca_data_collection.xlsx
+++ b/images/ca_data_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Desktop/MIDS_TPG/W210/capstone_fall20_irrigation/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F1222A-18F5-5846-945C-4EF56C4DEBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425ABE6C-C04E-934C-814F-DB68CEDBE53F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="1360" windowWidth="36260" windowHeight="28340" activeTab="2" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
+    <workbookView xWindow="57340" yWindow="8460" windowWidth="36260" windowHeight="26680" activeTab="2" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
   </bookViews>
   <sheets>
     <sheet name="CA_Data_Collection" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
   <si>
     <t>LATITUDE</t>
   </si>
@@ -135,13 +135,98 @@
   </si>
   <si>
     <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - H2@128</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - 0.20 Shift</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - 0.10 Shift</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - Top Layer FT</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - Full FT - 1e-5</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - FT PH - 1e-5</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - FT PH (half) - 1e-5</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - FT PH (half) - 5e-5</t>
+  </si>
+  <si>
+    <r>
+      <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity -  20%</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Zoom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity -  40%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Zoom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity -  40%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Zoom</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 90 rot</t>
+    </r>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - 0.1 Temp</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - 0.3 Temp</t>
+  </si>
+  <si>
+    <t>SimCLR Pretrain (20% training set) and Finetuned - 3% Positive Class - 50% Intensity - 0.3 Temp - 40% Zoom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,6 +247,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,13 +288,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +557,10 @@
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91</c:v>
+                  <c:v>0.91400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.91500000000000004</c:v>
+                  <c:v>0.91600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.8</c:v>
@@ -1702,7 +1801,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView topLeftCell="A32" zoomScale="135" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2593,15 +2692,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BC90CD-1B1D-A349-9236-A951D1CE880F}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2634,7 +2733,7 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>0.91</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2642,7 +2741,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.91500000000000004</v>
+        <v>0.91600000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2709,7 +2808,112 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>0.90400000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding tsne plotting for qualitative evaluation
</commit_message>
<xml_diff>
--- a/images/ca_data_collection.xlsx
+++ b/images/ca_data_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Desktop/MIDS_TPG/W210/capstone_fall20_irrigation/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E50048-50D4-0A46-91BA-C2FECB9F442D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215A2AF2-7D3E-1B49-B1DD-A5CF8306DBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62560" yWindow="11880" windowWidth="30380" windowHeight="19240" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
+    <workbookView xWindow="62540" yWindow="11880" windowWidth="30380" windowHeight="19240" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
   </bookViews>
   <sheets>
     <sheet name="CA_Data_Collection" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="91">
   <si>
     <t>LATITUDE</t>
   </si>
@@ -5001,8 +5001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B11D730-724F-C64E-B450-810506062CA1}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6179,7 +6179,10 @@
         <v>-121.375</v>
       </c>
       <c r="C70" t="s">
-        <v>89</v>
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -6218,7 +6221,10 @@
         <v>-122.125</v>
       </c>
       <c r="C73" t="s">
-        <v>89</v>
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -6231,6 +6237,9 @@
       <c r="C74" t="s">
         <v>89</v>
       </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -6268,7 +6277,10 @@
         <v>-122.125</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -6313,7 +6325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>39.625</v>
       </c>
@@ -6327,7 +6339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>39.875</v>
       </c>
@@ -6337,8 +6349,11 @@
       <c r="C82" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>39.875</v>
       </c>
@@ -6352,7 +6367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>39.875</v>
       </c>
@@ -6366,7 +6381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>39.875</v>
       </c>
@@ -6376,8 +6391,14 @@
       <c r="C85" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>32.625</v>
       </c>
@@ -6388,7 +6409,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>32.625</v>
       </c>
@@ -6399,7 +6420,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>32.625</v>
       </c>
@@ -6410,7 +6431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>32.625</v>
       </c>
@@ -6421,7 +6442,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>32.875</v>
       </c>
@@ -6432,7 +6453,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>32.875</v>
       </c>
@@ -6443,7 +6464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>32.875</v>
       </c>
@@ -6454,7 +6475,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>32.875</v>
       </c>
@@ -6465,7 +6486,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>33.125</v>
       </c>
@@ -6476,7 +6497,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>33.125</v>
       </c>
@@ -6487,7 +6508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>33.125</v>
       </c>

</xml_diff>

<commit_message>
adding some html images
</commit_message>
<xml_diff>
--- a/images/ca_data_collection.xlsx
+++ b/images/ca_data_collection.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Desktop/MIDS_TPG/W210/capstone_fall20_irrigation/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215A2AF2-7D3E-1B49-B1DD-A5CF8306DBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7B18CD-0936-0E4C-B723-83E3D86C4215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62540" yWindow="11880" windowWidth="30380" windowHeight="19240" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
+    <workbookView xWindow="10240" yWindow="3520" windowWidth="36940" windowHeight="19240" activeTab="5" xr2:uid="{BDD5E030-342C-6246-AA44-B5823F365658}"/>
   </bookViews>
   <sheets>
     <sheet name="CA_Data_Collection" sheetId="1" r:id="rId1"/>
     <sheet name="ValidationAUC" sheetId="3" r:id="rId2"/>
     <sheet name="ScatterPlot" sheetId="5" r:id="rId3"/>
-    <sheet name="BarChart" sheetId="6" r:id="rId4"/>
-    <sheet name="SimpleTable" sheetId="4" r:id="rId5"/>
-    <sheet name="Sensitivities" sheetId="2" r:id="rId6"/>
+    <sheet name="Sensitivities" sheetId="2" r:id="rId4"/>
+    <sheet name="BarChart" sheetId="6" r:id="rId5"/>
+    <sheet name="SimpleTable" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="93">
   <si>
     <t>LATITUDE</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>MARIA</t>
+  </si>
+  <si>
+    <t>CA18A50T1- Finetuned with BEN Data - BS64 -  5e-5</t>
+  </si>
+  <si>
+    <t>CA18A50T1- Finetuned with BEN Data - BS32-  5e-5</t>
   </si>
 </sst>
 </file>
@@ -5001,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B11D730-724F-C64E-B450-810506062CA1}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView topLeftCell="A67" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6325,7 +6331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>39.625</v>
       </c>
@@ -6339,7 +6345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>39.875</v>
       </c>
@@ -6353,7 +6359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>39.875</v>
       </c>
@@ -6367,7 +6373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>39.875</v>
       </c>
@@ -6381,7 +6387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>39.875</v>
       </c>
@@ -6394,11 +6400,8 @@
       <c r="D85" t="s">
         <v>13</v>
       </c>
-      <c r="E85" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>32.625</v>
       </c>
@@ -6409,7 +6412,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>32.625</v>
       </c>
@@ -6420,7 +6423,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>32.625</v>
       </c>
@@ -6431,7 +6434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>32.625</v>
       </c>
@@ -6442,7 +6445,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>32.875</v>
       </c>
@@ -6453,7 +6456,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>32.875</v>
       </c>
@@ -6464,7 +6467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>32.875</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>32.875</v>
       </c>
@@ -6486,7 +6489,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>33.125</v>
       </c>
@@ -6497,7 +6500,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>33.125</v>
       </c>
@@ -6508,7 +6511,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>33.125</v>
       </c>
@@ -6537,11 +6540,728 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BC90CD-1B1D-A349-9236-A951D1CE880F}">
+  <dimension ref="A1:E93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93:D93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="96.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>0.90400000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="7">
+        <v>0.91902399999999995</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.8972</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="7">
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.91690000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="7">
+        <v>0.89549999999999996</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="7">
+        <v>0.89770000000000005</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0.91390000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="7">
+        <v>0.89490000000000003</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="7">
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="7">
+        <v>0.90139999999999998</v>
+      </c>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="7">
+        <v>0.89880000000000004</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0.89690000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="7">
+        <v>0.8992</v>
+      </c>
+      <c r="C75" s="7">
+        <v>0.91255799999999998</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0.91705999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="7">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="C76" s="7">
+        <v>0.91566999999999998</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.91879999999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="7">
+        <v>0.89798599999999995</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D77" s="7">
+        <v>0.91679999999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="7">
+        <v>0.89729999999999999</v>
+      </c>
+      <c r="C78" s="7">
+        <v>0.91180000000000005</v>
+      </c>
+      <c r="D78" s="7">
+        <v>0.91605999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="7">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D79" s="7">
+        <v>0.91749999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="7">
+        <v>0.89459999999999995</v>
+      </c>
+      <c r="C80" s="7">
+        <v>0.91149999999999998</v>
+      </c>
+      <c r="D80" s="7">
+        <v>0.9163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81" s="7">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0.91259999999999997</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0.91549999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" s="7">
+        <v>0.89370000000000005</v>
+      </c>
+      <c r="C82" s="7">
+        <v>0.91110000000000002</v>
+      </c>
+      <c r="D82" s="7">
+        <v>0.91879999999999995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="7">
+        <v>0.89529999999999998</v>
+      </c>
+      <c r="C83" s="7">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="D83" s="7">
+        <v>0.91510000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87">
+        <v>0.89275000000000004</v>
+      </c>
+      <c r="C87">
+        <v>0.91290000000000004</v>
+      </c>
+      <c r="D87">
+        <v>0.91439999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" t="s">
+        <v>78</v>
+      </c>
+      <c r="D89" t="s">
+        <v>77</v>
+      </c>
+      <c r="E89">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="C90">
+        <v>0.914157</v>
+      </c>
+      <c r="D90">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="E90">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B92" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>70</v>
+      </c>
+      <c r="B93">
+        <v>0.90190000000000003</v>
+      </c>
+      <c r="C93">
+        <v>0.9143</v>
+      </c>
+      <c r="D93">
+        <v>0.93220000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667A3AE2-AF9E-0C45-A289-E5DFD881FFDB}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6554,9 +7274,10 @@
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="13" max="14" width="45.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>62</v>
       </c>
@@ -6590,8 +7311,14 @@
       <c r="L1" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -6630,7 +7357,7 @@
         <v>0.95189999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -6663,7 +7390,7 @@
         <v>0.94740000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -6695,8 +7422,11 @@
       <c r="J4" s="11">
         <v>0.92989999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M4" s="8">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -6728,8 +7458,11 @@
       <c r="J5" s="11">
         <v>0.91269999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M5" s="8">
+        <v>0.91010000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -6761,8 +7494,11 @@
       <c r="J6" s="11">
         <v>0.90390000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M6" s="8">
+        <v>0.9012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>86</v>
       </c>
@@ -6776,7 +7512,7 @@
         <v>0.93220000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>128</v>
       </c>
@@ -6787,7 +7523,7 @@
         <v>0.8508</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>32</v>
       </c>
@@ -6801,721 +7537,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BC90CD-1B1D-A349-9236-A951D1CE880F}">
-  <dimension ref="A1:E93"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93:D93"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="96.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>0.97399999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3">
-        <v>0.96499999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>0.80200000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6">
-        <v>0.70099999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7">
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10">
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17">
-        <v>0.90900000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18">
-        <v>0.91300000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21">
-        <v>0.90500000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24">
-        <v>0.89900000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25">
-        <v>0.90400000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27">
-        <v>0.91100000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30">
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31">
-        <v>0.91100000000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36">
-        <v>0.95799999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38">
-        <v>0.91900000000000004</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39">
-        <v>0.91900000000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42">
-        <v>0.91500000000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45">
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="7">
-        <v>0.91902399999999995</v>
-      </c>
-      <c r="C50" s="7">
-        <v>0.8972</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0.91100000000000003</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="7">
-        <v>0.91679999999999995</v>
-      </c>
-      <c r="C51" s="7">
-        <v>0.83379999999999999</v>
-      </c>
-      <c r="D51" s="7">
-        <v>0.91690000000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="7">
-        <v>0.89549999999999996</v>
-      </c>
-      <c r="C52" s="7">
-        <v>0.91080000000000005</v>
-      </c>
-      <c r="D52" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="7">
-        <v>0.89770000000000005</v>
-      </c>
-      <c r="C53" s="7">
-        <v>0.91239999999999999</v>
-      </c>
-      <c r="D53" s="7">
-        <v>0.91390000000000005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="7">
-        <v>0.89490000000000003</v>
-      </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="7">
-        <v>0.90069999999999995</v>
-      </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="7">
-        <v>0.90139999999999998</v>
-      </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="7">
-        <v>0.89880000000000004</v>
-      </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="7">
-        <v>0.89690000000000003</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C74" t="s">
-        <v>78</v>
-      </c>
-      <c r="D74" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>66</v>
-      </c>
-      <c r="B75" s="7">
-        <v>0.8992</v>
-      </c>
-      <c r="C75" s="7">
-        <v>0.91255799999999998</v>
-      </c>
-      <c r="D75" s="7">
-        <v>0.91705999999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" s="7">
-        <v>0.89759999999999995</v>
-      </c>
-      <c r="C76" s="7">
-        <v>0.91566999999999998</v>
-      </c>
-      <c r="D76" s="7">
-        <v>0.91879999999999995</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="7">
-        <v>0.89798599999999995</v>
-      </c>
-      <c r="C77" s="7">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D77" s="7">
-        <v>0.91679999999999995</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" s="7">
-        <v>0.89729999999999999</v>
-      </c>
-      <c r="C78" s="7">
-        <v>0.91180000000000005</v>
-      </c>
-      <c r="D78" s="7">
-        <v>0.91605999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="7">
-        <v>0.90410000000000001</v>
-      </c>
-      <c r="C79" s="7">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D79" s="7">
-        <v>0.91749999999999998</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" s="7">
-        <v>0.89459999999999995</v>
-      </c>
-      <c r="C80" s="7">
-        <v>0.91149999999999998</v>
-      </c>
-      <c r="D80" s="7">
-        <v>0.9163</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="7">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="C81" s="7">
-        <v>0.91259999999999997</v>
-      </c>
-      <c r="D81" s="7">
-        <v>0.91549999999999998</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>73</v>
-      </c>
-      <c r="B82" s="7">
-        <v>0.89370000000000005</v>
-      </c>
-      <c r="C82" s="7">
-        <v>0.91110000000000002</v>
-      </c>
-      <c r="D82" s="7">
-        <v>0.91879999999999995</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>74</v>
-      </c>
-      <c r="B83" s="7">
-        <v>0.89529999999999998</v>
-      </c>
-      <c r="C83" s="7">
-        <v>0.91749999999999998</v>
-      </c>
-      <c r="D83" s="7">
-        <v>0.91510000000000002</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" t="s">
-        <v>76</v>
-      </c>
-      <c r="C86" t="s">
-        <v>78</v>
-      </c>
-      <c r="D86" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>70</v>
-      </c>
-      <c r="B87">
-        <v>0.89275000000000004</v>
-      </c>
-      <c r="C87">
-        <v>0.91290000000000004</v>
-      </c>
-      <c r="D87">
-        <v>0.91439999999999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>82</v>
-      </c>
-      <c r="B89" t="s">
-        <v>76</v>
-      </c>
-      <c r="C89" t="s">
-        <v>78</v>
-      </c>
-      <c r="D89" t="s">
-        <v>77</v>
-      </c>
-      <c r="E89">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>70</v>
-      </c>
-      <c r="B90">
-        <v>0.90390000000000004</v>
-      </c>
-      <c r="C90">
-        <v>0.914157</v>
-      </c>
-      <c r="D90">
-        <v>0.91659999999999997</v>
-      </c>
-      <c r="E90">
-        <v>0.94399999999999995</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>82</v>
-      </c>
-      <c r="B92" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" t="s">
-        <v>78</v>
-      </c>
-      <c r="D92">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>70</v>
-      </c>
-      <c r="B93">
-        <v>0.90190000000000003</v>
-      </c>
-      <c r="C93">
-        <v>0.9143</v>
-      </c>
-      <c r="D93">
-        <v>0.93220000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>